<commit_message>
checking if shape in bidaf-pytorch matches with bi-att-flow tf
</commit_message>
<xml_diff>
--- a/tf-pt-shape-analysis.xlsx
+++ b/tf-pt-shape-analysis.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="8580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,6 +25,140 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+  <si>
+    <t>opts</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>in_height</t>
+  </si>
+  <si>
+    <t>in_width</t>
+  </si>
+  <si>
+    <t>in_channels</t>
+  </si>
+  <si>
+    <t>filter_height</t>
+  </si>
+  <si>
+    <t>filter_width</t>
+  </si>
+  <si>
+    <t>out_channels</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Acx</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>JX</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N * M </t>
+  </si>
+  <si>
+    <t xml:space="preserve">W </t>
+  </si>
+  <si>
+    <t>in_</t>
+  </si>
+  <si>
+    <t>filter_size</t>
+  </si>
+  <si>
+    <t>filter_</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>N (60)</t>
+  </si>
+  <si>
+    <t>M (100)</t>
+  </si>
+  <si>
+    <t>JX (50)</t>
+  </si>
+  <si>
+    <t>W (50)</t>
+  </si>
+  <si>
+    <t>dc (8)</t>
+  </si>
+  <si>
+    <t>strides</t>
+  </si>
+  <si>
+    <t>1,1,1,1</t>
+  </si>
+  <si>
+    <t>paddings</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>Acx_</t>
+  </si>
+  <si>
+    <t>Acq_</t>
+  </si>
+  <si>
+    <t>Acx_orig</t>
+  </si>
+  <si>
+    <t>Acq_orig</t>
+  </si>
+  <si>
+    <t>qq_</t>
+  </si>
+  <si>
+    <t>xx_orig</t>
+  </si>
+  <si>
+    <t>qq_orig</t>
+  </si>
+  <si>
+    <t>JQ</t>
+  </si>
+  <si>
+    <t>N * M</t>
+  </si>
+  <si>
+    <t>xx_ (filter_sizes = 100,  filter_heights = 5)</t>
+  </si>
+  <si>
+    <t>JX (sent_size)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -53,12 +188,137 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +596,566 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="10.83203125" style="6"/>
+    <col min="6" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="13.6640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2">
+        <v>100</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E3" s="6">
+        <v>6000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9">
+        <v>6000</v>
+      </c>
+      <c r="K4" s="9">
+        <v>50</v>
+      </c>
+      <c r="L4" s="9">
+        <v>50</v>
+      </c>
+      <c r="M4" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2">
+        <v>100</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I6" s="8"/>
+      <c r="J6" s="9">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9">
+        <v>5</v>
+      </c>
+      <c r="L6" s="12">
+        <v>8</v>
+      </c>
+      <c r="M6" s="10">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="10.83203125" style="2"/>
+    <col min="11" max="14" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="10.83203125" style="2"/>
+    <col min="16" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="10.83203125" style="2"/>
+    <col min="21" max="24" width="10.83203125" style="1"/>
+    <col min="25" max="25" width="10.83203125" style="2"/>
+    <col min="26" max="29" width="10.83203125" style="1"/>
+    <col min="30" max="30" width="10.83203125" style="2"/>
+    <col min="31" max="34" width="10.83203125" style="1"/>
+    <col min="35" max="35" width="10.83203125" style="2"/>
+    <col min="36" max="39" width="10.83203125" style="1"/>
+    <col min="40" max="40" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="14"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="X2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="15"/>
+      <c r="AN2" s="16"/>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>161</v>
+      </c>
+      <c r="D3" s="7">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2">
+        <v>8</v>
+      </c>
+      <c r="F3" s="7">
+        <v>60</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>161</v>
+      </c>
+      <c r="I3" s="7">
+        <v>100</v>
+      </c>
+      <c r="K3" s="7">
+        <v>60</v>
+      </c>
+      <c r="L3" s="7">
+        <v>20</v>
+      </c>
+      <c r="M3" s="7">
+        <v>16</v>
+      </c>
+      <c r="N3" s="7">
+        <v>8</v>
+      </c>
+      <c r="P3" s="7">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>20</v>
+      </c>
+      <c r="R3" s="7">
+        <v>100</v>
+      </c>
+      <c r="U3" s="7">
+        <v>60</v>
+      </c>
+      <c r="V3" s="7">
+        <v>161</v>
+      </c>
+      <c r="W3" s="7">
+        <v>16</v>
+      </c>
+      <c r="X3" s="7">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="7">
+        <v>60</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="7">
+        <v>16</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="7">
+        <v>60</v>
+      </c>
+      <c r="AF3" s="7">
+        <v>161</v>
+      </c>
+      <c r="AG3" s="7">
+        <v>100</v>
+      </c>
+      <c r="AJ3" s="7">
+        <v>60</v>
+      </c>
+      <c r="AK3" s="7">
+        <v>20</v>
+      </c>
+      <c r="AL3" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>60</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>76</v>
+      </c>
+      <c r="D4" s="7">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+      <c r="F4" s="7">
+        <v>60</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>76</v>
+      </c>
+      <c r="I4" s="7">
+        <v>100</v>
+      </c>
+      <c r="K4" s="7">
+        <v>60</v>
+      </c>
+      <c r="L4" s="7">
+        <v>24</v>
+      </c>
+      <c r="M4" s="7">
+        <v>16</v>
+      </c>
+      <c r="N4" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>134</v>
+      </c>
+      <c r="D5" s="7">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7">
+        <v>60</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>134</v>
+      </c>
+      <c r="I5" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>60</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>258</v>
+      </c>
+      <c r="D6" s="7">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="7">
+        <v>60</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>258</v>
+      </c>
+      <c r="I6" s="7">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed conv2d issue. by default, conv2d in pytorch uses dilation=1, whereas tensorflow doesn't use any dilation.
</commit_message>
<xml_diff>
--- a/tf-pt-shape-analysis.xlsx
+++ b/tf-pt-shape-analysis.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>opts</t>
   </si>
@@ -150,13 +150,58 @@
     <t>JQ</t>
   </si>
   <si>
-    <t>N * M</t>
-  </si>
-  <si>
     <t>xx_ (filter_sizes = 100,  filter_heights = 5)</t>
   </si>
   <si>
     <t>JX (sent_size)</t>
+  </si>
+  <si>
+    <t>stride = 1</t>
+  </si>
+  <si>
+    <t>N * M (batch)</t>
+  </si>
+  <si>
+    <t>JX (in_height)</t>
+  </si>
+  <si>
+    <t>W (in_width)</t>
+  </si>
+  <si>
+    <t>dc (in_channels)</t>
+  </si>
+  <si>
+    <t>C_in</t>
+  </si>
+  <si>
+    <t>H_in</t>
+  </si>
+  <si>
+    <t>W_in</t>
+  </si>
+  <si>
+    <t>torch:</t>
+  </si>
+  <si>
+    <t>padding</t>
+  </si>
+  <si>
+    <t>dilation</t>
+  </si>
+  <si>
+    <t>kernel_size[0]</t>
+  </si>
+  <si>
+    <t>kernel_size[1]</t>
+  </si>
+  <si>
+    <t>H_out</t>
+  </si>
+  <si>
+    <t>W_out</t>
+  </si>
+  <si>
+    <t>C_out</t>
   </si>
 </sst>
 </file>
@@ -293,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -317,6 +362,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -794,33 +845,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AR9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="9" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="2"/>
-    <col min="11" max="14" width="10.83203125" style="1"/>
-    <col min="15" max="15" width="10.83203125" style="2"/>
-    <col min="16" max="19" width="10.83203125" style="1"/>
-    <col min="20" max="20" width="10.83203125" style="2"/>
-    <col min="21" max="24" width="10.83203125" style="1"/>
-    <col min="25" max="25" width="10.83203125" style="2"/>
-    <col min="26" max="29" width="10.83203125" style="1"/>
-    <col min="30" max="30" width="10.83203125" style="2"/>
-    <col min="31" max="34" width="10.83203125" style="1"/>
-    <col min="35" max="35" width="10.83203125" style="2"/>
-    <col min="36" max="39" width="10.83203125" style="1"/>
-    <col min="40" max="40" width="10.83203125" style="2"/>
+    <col min="11" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="15.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="6"/>
+    <col min="17" max="18" width="10.83203125" style="1"/>
+    <col min="19" max="19" width="13" style="2" customWidth="1"/>
+    <col min="20" max="23" width="10.83203125" style="1"/>
+    <col min="24" max="24" width="10.83203125" style="2"/>
+    <col min="25" max="28" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="10.83203125" style="2"/>
+    <col min="30" max="33" width="10.83203125" style="1"/>
+    <col min="34" max="34" width="10.83203125" style="2"/>
+    <col min="35" max="38" width="10.83203125" style="1"/>
+    <col min="39" max="39" width="10.83203125" style="2"/>
+    <col min="40" max="43" width="10.83203125" style="1"/>
+    <col min="44" max="44" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>32</v>
       </c>
@@ -836,49 +894,55 @@
       <c r="I1" s="13"/>
       <c r="J1" s="14"/>
       <c r="K1" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L1" s="13"/>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="14"/>
-      <c r="P1" s="13" t="s">
-        <v>37</v>
+      <c r="P1" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="S1" s="14"/>
+      <c r="T1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="13"/>
       <c r="V1" s="13"/>
       <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="13" t="s">
-        <v>38</v>
-      </c>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="13"/>
       <c r="AA1" s="13"/>
       <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1" s="13"/>
       <c r="AF1" s="13"/>
       <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="14"/>
-      <c r="AJ1" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ1" s="13"/>
       <c r="AK1" s="13"/>
       <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="14"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>10</v>
       </c>
@@ -886,7 +950,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>15</v>
@@ -895,16 +959,16 @@
         <v>16</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="15"/>
@@ -912,49 +976,61 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="15" t="s">
+      <c r="P2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="Z2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="AA2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="15" t="s">
+      <c r="AB2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="15" t="s">
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="AF2" s="15" t="s">
+      <c r="AJ2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AK2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AH2" s="15" t="s">
+      <c r="AL2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="16"/>
+      <c r="AM2" s="16"/>
+      <c r="AN2" s="15"/>
+      <c r="AO2" s="15"/>
+      <c r="AP2" s="15"/>
+      <c r="AQ2" s="15"/>
+      <c r="AR2" s="16"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>60</v>
       </c>
@@ -991,62 +1067,74 @@
       <c r="M3" s="7">
         <v>100</v>
       </c>
-      <c r="P3" s="7">
-        <v>60</v>
+      <c r="P3" s="6">
+        <v>1</v>
       </c>
       <c r="Q3" s="7">
+        <v>5</v>
+      </c>
+      <c r="R3" s="7">
+        <v>8</v>
+      </c>
+      <c r="S3" s="2">
+        <v>100</v>
+      </c>
+      <c r="T3" s="7">
+        <v>60</v>
+      </c>
+      <c r="U3" s="7">
         <v>1</v>
       </c>
-      <c r="R3" s="7">
+      <c r="V3" s="7">
         <v>161</v>
       </c>
-      <c r="S3" s="7">
+      <c r="W3" s="7">
         <v>100</v>
       </c>
-      <c r="U3" s="7">
-        <v>60</v>
-      </c>
-      <c r="V3" s="7">
+      <c r="Y3" s="7">
+        <v>60</v>
+      </c>
+      <c r="Z3" s="7">
         <v>20</v>
       </c>
-      <c r="W3" s="7">
+      <c r="AA3" s="7">
         <v>16</v>
       </c>
-      <c r="X3" s="7">
+      <c r="AB3" s="7">
         <v>8</v>
       </c>
-      <c r="Z3" s="7">
-        <v>60</v>
-      </c>
-      <c r="AA3" s="7">
+      <c r="AD3" s="7">
+        <v>60</v>
+      </c>
+      <c r="AE3" s="7">
         <v>20</v>
       </c>
-      <c r="AB3" s="7">
+      <c r="AF3" s="7">
         <v>100</v>
       </c>
-      <c r="AE3" s="7">
-        <v>60</v>
-      </c>
-      <c r="AF3" s="7">
+      <c r="AI3" s="7">
+        <v>60</v>
+      </c>
+      <c r="AJ3" s="7">
         <v>20</v>
       </c>
-      <c r="AG3" s="7">
+      <c r="AK3" s="7">
         <v>16</v>
       </c>
-      <c r="AH3" s="7">
+      <c r="AL3" s="7">
         <v>8</v>
       </c>
-      <c r="AJ3" s="7">
-        <v>60</v>
-      </c>
-      <c r="AK3" s="7">
+      <c r="AN3" s="7">
+        <v>60</v>
+      </c>
+      <c r="AO3" s="7">
         <v>20</v>
       </c>
-      <c r="AL3" s="7">
+      <c r="AP3" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>60</v>
       </c>
@@ -1062,32 +1150,47 @@
       <c r="E4" s="2">
         <v>8</v>
       </c>
-      <c r="P4" s="7">
-        <v>60</v>
-      </c>
-      <c r="Q4" s="7">
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="7">
+        <v>60</v>
+      </c>
+      <c r="U4" s="7">
         <v>1</v>
       </c>
-      <c r="R4" s="7">
+      <c r="V4" s="7">
         <v>76</v>
       </c>
-      <c r="S4" s="7">
+      <c r="W4" s="7">
         <v>100</v>
       </c>
-      <c r="U4" s="7">
-        <v>60</v>
-      </c>
-      <c r="V4" s="7">
+      <c r="Y4" s="7">
+        <v>60</v>
+      </c>
+      <c r="Z4" s="7">
         <v>24</v>
       </c>
-      <c r="W4" s="7">
+      <c r="AA4" s="7">
         <v>16</v>
       </c>
-      <c r="X4" s="7">
+      <c r="AB4" s="7">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -1103,20 +1206,32 @@
       <c r="E5" s="2">
         <v>8</v>
       </c>
-      <c r="P5" s="7">
-        <v>60</v>
-      </c>
-      <c r="Q5" s="7">
+      <c r="K5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="7">
+        <v>60</v>
+      </c>
+      <c r="U5" s="7">
         <v>1</v>
       </c>
-      <c r="R5" s="7">
+      <c r="V5" s="7">
         <v>134</v>
       </c>
-      <c r="S5" s="7">
+      <c r="W5" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>60</v>
       </c>
@@ -1132,29 +1247,74 @@
       <c r="E6" s="2">
         <v>8</v>
       </c>
-      <c r="P6" s="7">
-        <v>60</v>
-      </c>
-      <c r="Q6" s="7">
+      <c r="K6" s="1">
+        <v>60</v>
+      </c>
+      <c r="L6" s="1">
+        <v>100</v>
+      </c>
+      <c r="M6" s="1">
+        <f>_xlfn.FLOOR.MATH((G3 + 2 * L9 - M9 * (N9 - 1) - 1) / 1 + 1)</f>
+        <v>161</v>
+      </c>
+      <c r="N6" s="1">
+        <f>_xlfn.FLOOR.MATH((H3 + 2 * L9 - M9 * (O9 - 1) - 1) / 1 + 1)</f>
+        <v>16</v>
+      </c>
+      <c r="T6" s="7">
+        <v>60</v>
+      </c>
+      <c r="U6" s="7">
         <v>1</v>
       </c>
-      <c r="R6" s="7">
+      <c r="V6" s="7">
         <v>258</v>
       </c>
-      <c r="S6" s="7">
+      <c r="W6" s="7">
         <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="L8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <f>P3</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="2">
+        <f>Q3</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="Z1:AD1"/>
+  <mergeCells count="9">
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="P1:S1"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Y1:AC1"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="AI1:AM1"/>
     <mergeCell ref="K1:O1"/>
-    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AN1:AR1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
doc doesn't match output?
</commit_message>
<xml_diff>
--- a/tf-pt-shape-analysis.xlsx
+++ b/tf-pt-shape-analysis.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>opts</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>W_in</t>
-  </si>
-  <si>
-    <t>torch:</t>
   </si>
   <si>
     <t>padding</t>
@@ -845,10 +842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR9"/>
+  <dimension ref="A1:AR11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1207,16 +1204,16 @@
         <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="T5" s="7">
         <v>60</v>
@@ -1276,16 +1273,16 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="L8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
@@ -1302,6 +1299,34 @@
       <c r="O9" s="2">
         <f>Q3</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="K10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="K11" s="7">
+        <v>60</v>
+      </c>
+      <c r="L11" s="7">
+        <v>161</v>
+      </c>
+      <c r="M11" s="7">
+        <v>16</v>
+      </c>
+      <c r="N11" s="7">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need to implement the logits function using TriLinear
</commit_message>
<xml_diff>
--- a/tf-pt-shape-analysis.xlsx
+++ b/tf-pt-shape-analysis.xlsx
@@ -349,22 +349,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -876,156 +876,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="13" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="13" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="17" t="s">
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="13" t="s">
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="13" t="s">
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="13" t="s">
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="13" t="s">
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="13" t="s">
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="14"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="17"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="18" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="15" t="s">
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="Z2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AA2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="16"/>
-      <c r="AI2" s="15" t="s">
+      <c r="AB2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AJ2" s="15" t="s">
+      <c r="AJ2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AK2" s="15" t="s">
+      <c r="AK2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="AL2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM2" s="16"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="16"/>
+      <c r="AL2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="13"/>
+      <c r="AP2" s="13"/>
+      <c r="AQ2" s="13"/>
+      <c r="AR2" s="14"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1331,15 +1331,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="AI1:AM1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="AN1:AR1"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="AD1:AH1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="Y1:AC1"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="AI1:AM1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="AN1:AR1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>